<commit_message>
Added logic to handle null cells and 12hr to 24hr format
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmart\OneDrive\Desktop\MedicorDataFormatter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://medicorsoftware-my.sharepoint.com/personal/kris_medicorsoftware_com/Documents/Medicor/HR/Software dev Job Ad/Presentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF61B0A-D885-4CC7-86F3-E402C56C9EE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1DB53C1C-FD47-4BB3-BB48-F7AD535890F0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10808" xr2:uid="{1DB53C1C-FD47-4BB3-BB48-F7AD535890F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Time of anaesthetic start</t>
   </si>
@@ -44,6 +43,18 @@
   <si>
     <t>Time into Recovery</t>
   </si>
+  <si>
+    <t>Time Out of Recovery</t>
+  </si>
+  <si>
+    <t>Time of Anaesthetic Start</t>
+  </si>
+  <si>
+    <t>Time into Theatre</t>
+  </si>
+  <si>
+    <t>Time out of Theatre</t>
+  </si>
 </sst>
 </file>
 
@@ -52,7 +63,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,15 +88,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000" tint="0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFF0000" tint="0"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000" tint="0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000" tint="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,23 +427,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8EA0C53-A141-40AA-B759-62088F3C5F05}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" style="2" customWidth="1"/>
-    <col min="2" max="3" width="17.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="21.88671875" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="20.46484375" customWidth="1" style="2"/>
+    <col min="2" max="2" bestFit="1" width="14.53125" customWidth="1" style="2"/>
+    <col min="3" max="3" bestFit="1" width="14.9296875" customWidth="1" style="2"/>
+    <col min="4" max="4" bestFit="1" width="15.53125" customWidth="1" style="2"/>
+    <col min="5" max="5" bestFit="1" width="16.1328125" customWidth="1" style="2"/>
+    <col min="6" max="6" bestFit="1" width="15.86328125" customWidth="1" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,25 +463,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="B2" s="1">
-        <v>42364.648611111108</v>
+        <v>42364.64861111111</v>
       </c>
       <c r="C2" s="1">
-        <v>42364.661805555559</v>
+        <v>42364.66180555556</v>
       </c>
       <c r="D2" s="1">
-        <v>42364.675694444442</v>
+        <v>42364.67569444444</v>
       </c>
       <c r="E2" s="1">
-        <v>42364.686805555553</v>
-      </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>42364.68680555555</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="1">
-        <v>42586.486111111109</v>
+        <v>42586.48611111111</v>
       </c>
       <c r="B3" s="1">
         <v>42586.5</v>
@@ -464,58 +494,58 @@
         <v>42586.5</v>
       </c>
       <c r="D3" s="1">
-        <v>42586.517361111109</v>
+        <v>42586.51736111111</v>
       </c>
       <c r="E3" s="1">
-        <v>42586.518750000003</v>
+        <v>42586.51875</v>
       </c>
       <c r="F3" s="1">
-        <v>42586.518750000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>42586.51875</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="1">
         <v>42557.413194444445</v>
       </c>
       <c r="B4" s="1">
-        <v>42557.418749999997</v>
+        <v>42557.41875</v>
       </c>
       <c r="C4" s="1">
-        <v>42557.422222222223</v>
+        <v>42557.42222222222</v>
       </c>
       <c r="D4" s="1">
         <v>42557.436111111114</v>
       </c>
       <c r="E4" s="1">
-        <v>42557.443055555559</v>
+        <v>42557.44305555556</v>
       </c>
       <c r="F4" s="1">
-        <v>42557.443749999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>42557.44375</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="1">
-        <v>42671.527777777781</v>
-      </c>
-      <c r="B5" s="1">
-        <v>42671.068055555559</v>
+        <v>42671.52777777778</v>
+      </c>
+      <c r="B5" s="3">
+        <v>42671.56805555556</v>
       </c>
       <c r="C5" s="1">
-        <v>42671.571527777778</v>
+        <v>42671.57152777778</v>
       </c>
       <c r="D5" s="1">
-        <v>42671.630555555559</v>
-      </c>
-      <c r="E5" s="1">
-        <v>42671.140972222223</v>
+        <v>42671.63055555556</v>
+      </c>
+      <c r="E5" s="3">
+        <v>42671.64097222222</v>
       </c>
       <c r="F5" s="1">
-        <v>42671.642361111109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>42670.09652777778</v>
+        <v>42671.64236111111</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>42670.59652777778</v>
       </c>
       <c r="B6" s="1">
         <v>42670.606944444444</v>
@@ -527,24 +557,24 @@
         <v>42670.634722222225</v>
       </c>
       <c r="E6" s="1">
-        <v>42670.652777777781</v>
+        <v>42670.65277777778</v>
       </c>
       <c r="F6" s="1">
         <v>42670.654861111114</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7">
       <c r="A7" s="1">
-        <v>42720.442361111112</v>
+        <v>42720.44236111111</v>
       </c>
       <c r="B7" s="1">
-        <v>42720.454861111109</v>
+        <v>42720.45486111111</v>
       </c>
       <c r="C7" s="1">
         <v>42720.458333333336</v>
       </c>
       <c r="D7" s="1">
-        <v>42720.522916666669</v>
+        <v>42720.52291666667</v>
       </c>
       <c r="E7" s="1">
         <v>42720.532638888886</v>
@@ -553,88 +583,92 @@
         <v>42720.53402777778</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8">
       <c r="A8" s="1">
-        <v>42405.518750000003</v>
+        <v>42405.51875</v>
       </c>
       <c r="B8" s="1">
-        <v>42405.519444444442</v>
+        <v>42405.51944444444</v>
       </c>
       <c r="C8" s="1">
-        <v>42405.520138888889</v>
+        <v>42405.52013888889</v>
       </c>
       <c r="D8" s="1">
-        <v>42405.533333333333</v>
+        <v>42405.53333333333</v>
       </c>
       <c r="E8" s="1">
-        <v>42405.550694444442</v>
+        <v>42405.55069444444</v>
       </c>
       <c r="F8" s="1">
         <v>42405.552777777775</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9">
       <c r="A9" s="1">
         <v>42408.21597222222</v>
       </c>
       <c r="B9" s="1">
-        <v>42408.216666666667</v>
+        <v>42408.21666666667</v>
       </c>
       <c r="C9" s="1">
-        <v>42408.230555555558</v>
+        <v>42408.23055555556</v>
       </c>
       <c r="D9" s="1">
-        <v>42408.267361111109</v>
+        <v>42408.26736111111</v>
       </c>
       <c r="E9" s="1">
-        <v>42408.290277777778</v>
-      </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>42408.29027777778</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" s="1">
-        <v>42442.722222222219</v>
+        <v>42442.72222222222</v>
       </c>
       <c r="B10" s="1">
-        <v>42442.752083333333</v>
+        <v>42442.75208333333</v>
       </c>
       <c r="C10" s="1">
-        <v>42442.755555555559</v>
+        <v>42442.75555555556</v>
       </c>
       <c r="D10" s="1">
-        <v>42442.790277777778</v>
+        <v>42442.79027777778</v>
       </c>
       <c r="E10" s="1">
         <v>42442.836805555555</v>
       </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" s="1">
-        <v>42464.434027777781</v>
+        <v>42464.43402777778</v>
       </c>
       <c r="B11" s="1">
         <v>42464.436111111114</v>
       </c>
       <c r="C11" s="1">
-        <v>42464.438194444447</v>
+        <v>42464.43819444445</v>
       </c>
       <c r="D11" s="1">
         <v>42464.447916666664</v>
       </c>
       <c r="E11" s="1">
-        <v>42464.459722222222</v>
+        <v>42464.45972222222</v>
       </c>
       <c r="F11" s="1">
-        <v>42464.459722222222</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>42464.45972222222</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" s="1">
         <v>42464.399305555555</v>
       </c>
       <c r="B12" s="1">
-        <v>42464.405555555553</v>
+        <v>42464.40555555555</v>
       </c>
       <c r="C12" s="1">
         <v>42464.40625</v>
@@ -643,14 +677,16 @@
         <v>42464.415972222225</v>
       </c>
       <c r="E12" s="1">
-        <v>42464.422222222223</v>
+        <v>42464.42222222222</v>
       </c>
       <c r="F12" s="1">
-        <v>42464.422222222223</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+        <v>42464.42222222222</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="B13" s="1">
         <v>42464.381944444445</v>
       </c>
@@ -658,17 +694,16 @@
         <v>42464.381944444445</v>
       </c>
       <c r="D13" s="1">
-        <v>42464.382638888892</v>
+        <v>42464.38263888889</v>
       </c>
       <c r="E13" s="1">
-        <v>42464.382638888892</v>
+        <v>42464.38263888889</v>
       </c>
       <c r="F13" s="1">
         <v>42464.388194444444</v>
       </c>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14">
       <c r="A14" s="1">
         <v>42461.427083333336</v>
       </c>
@@ -679,7 +714,7 @@
         <v>42461.444444444445</v>
       </c>
       <c r="D14" s="1">
-        <v>42461.490972222222</v>
+        <v>42461.49097222222</v>
       </c>
       <c r="E14" s="1">
         <v>42461.5</v>
@@ -688,7 +723,7 @@
         <v>42461.501388888886</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15">
       <c r="A15" s="1">
         <v>42461.35833333333</v>
       </c>
@@ -699,36 +734,38 @@
         <v>42461.370833333334</v>
       </c>
       <c r="D15" s="1">
-        <v>42461.411805555559</v>
+        <v>42461.41180555556</v>
       </c>
       <c r="E15" s="1">
-        <v>42461.421527777777</v>
+        <v>42461.42152777778</v>
       </c>
       <c r="F15" s="1">
-        <v>42461.425000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>42461.425</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" s="1">
-        <v>42464.602083333331</v>
-      </c>
-      <c r="B16" s="1"/>
+        <v>42464.60208333333</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C16" s="1">
-        <v>42464.612500000003</v>
+        <v>42464.6125</v>
       </c>
       <c r="D16" s="1">
         <v>42464.666666666664</v>
       </c>
-      <c r="E16" s="1">
-        <v>42464.175000000003</v>
+      <c r="E16" s="3">
+        <v>42464.675</v>
       </c>
       <c r="F16" s="1">
-        <v>42464.675000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42464.675</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" s="1">
-        <v>42464.559027777781</v>
+        <v>42464.55902777778</v>
       </c>
       <c r="B17" s="1">
         <v>42464.5625</v>
@@ -740,58 +777,58 @@
         <v>42464.592361111114</v>
       </c>
       <c r="E17" s="1">
-        <v>42464.601388888892</v>
+        <v>42464.60138888889</v>
       </c>
       <c r="F17" s="1">
-        <v>42464.601388888892</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42464.60138888889</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18" s="1">
-        <v>42464.443055555559</v>
+        <v>42464.44305555556</v>
       </c>
       <c r="B18" s="1">
-        <v>42464.448611111111</v>
+        <v>42464.44861111111</v>
       </c>
       <c r="C18" s="1">
-        <v>42464.456944444442</v>
+        <v>42464.45694444444</v>
       </c>
       <c r="D18" s="1">
-        <v>42464.505555555559</v>
+        <v>42464.50555555556</v>
       </c>
       <c r="E18" s="1">
         <v>42464.513194444444</v>
       </c>
       <c r="F18" s="1">
-        <v>42464.513888888891</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42464.51388888889</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" s="1">
-        <v>42464.372916666667</v>
+        <v>42464.37291666667</v>
       </c>
       <c r="B19" s="1">
-        <v>42464.381249999999</v>
+        <v>42464.38125</v>
       </c>
       <c r="C19" s="1">
-        <v>42464.386111111111</v>
+        <v>42464.38611111111</v>
       </c>
       <c r="D19" s="1">
         <v>42464.436111111114</v>
       </c>
       <c r="E19" s="1">
-        <v>42464.438194444447</v>
+        <v>42464.43819444445</v>
       </c>
       <c r="F19" s="1">
-        <v>42464.439583333333</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42464.43958333333</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20" s="1">
         <v>42468.649305555555</v>
       </c>
       <c r="B20" s="1">
-        <v>42468.654166666667</v>
+        <v>42468.65416666667</v>
       </c>
       <c r="C20" s="1">
         <v>42468.65625</v>
@@ -806,7 +843,7 @@
         <v>42468.663194444445</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21">
       <c r="A21" s="1">
         <v>42468.615277777775</v>
       </c>
@@ -814,37 +851,39 @@
         <v>42468.629166666666</v>
       </c>
       <c r="C21" s="1">
-        <v>42468.629861111112</v>
+        <v>42468.62986111111</v>
       </c>
       <c r="D21" s="1">
         <v>42468.631944444445</v>
       </c>
       <c r="E21" s="1">
-        <v>42468.637499999997</v>
-      </c>
-      <c r="F21" s="1">
-        <v>42468.137499999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42468.6375</v>
+      </c>
+      <c r="F21" s="3">
+        <v>42468.6375</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" s="1">
         <v>42468.57708333333</v>
       </c>
       <c r="B22" s="1">
-        <v>42468.588888888888</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>42468.58888888889</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D22" s="1">
-        <v>42468.602083333331</v>
+        <v>42468.60208333333</v>
       </c>
       <c r="E22" s="1">
-        <v>42468.611111111109</v>
+        <v>42468.61111111111</v>
       </c>
       <c r="F22" s="1">
-        <v>42468.611111111109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42468.61111111111</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" s="1">
         <v>42467.472916666666</v>
       </c>
@@ -858,24 +897,24 @@
         <v>42467.501388888886</v>
       </c>
       <c r="E23" s="1">
-        <v>42467.503472222219</v>
+        <v>42467.50347222222</v>
       </c>
       <c r="F23" s="1">
-        <v>42467.504861111112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42467.50486111111</v>
+      </c>
+    </row>
+    <row r="24">
       <c r="A24" s="1">
         <v>42467.455555555556</v>
       </c>
       <c r="B24" s="1">
-        <v>42467.456250000003</v>
+        <v>42467.45625</v>
       </c>
       <c r="C24" s="1">
-        <v>42467.456944444442</v>
+        <v>42467.45694444444</v>
       </c>
       <c r="D24" s="1">
-        <v>42467.461111111108</v>
+        <v>42467.46111111111</v>
       </c>
       <c r="E24" s="1">
         <v>42467.464583333334</v>
@@ -884,29 +923,29 @@
         <v>42467.464583333334</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25">
       <c r="A25" s="1">
         <v>42467.424305555556</v>
       </c>
       <c r="B25" s="1">
-        <v>42467.431250000001</v>
+        <v>42467.43125</v>
       </c>
       <c r="C25" s="1">
-        <v>42467.434027777781</v>
+        <v>42467.43402777778</v>
       </c>
       <c r="D25" s="1">
-        <v>42467.445138888892</v>
+        <v>42467.44513888889</v>
       </c>
       <c r="E25" s="1">
-        <v>42467.448611111111</v>
+        <v>42467.44861111111</v>
       </c>
       <c r="F25" s="1">
-        <v>42467.448611111111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42467.44861111111</v>
+      </c>
+    </row>
+    <row r="26">
       <c r="A26" s="1">
-        <v>42467.397222222222</v>
+        <v>42467.39722222222</v>
       </c>
       <c r="B26" s="1">
         <v>42467.40347222222</v>
@@ -918,38 +957,38 @@
         <v>42467.415972222225</v>
       </c>
       <c r="E26" s="1">
-        <v>42467.418749999997</v>
+        <v>42467.41875</v>
       </c>
       <c r="F26" s="1">
         <v>42467.419444444444</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27">
       <c r="A27" s="1">
-        <v>42467.673611111109</v>
+        <v>42467.67361111111</v>
       </c>
       <c r="B27" s="1">
-        <v>42467.678472222222</v>
+        <v>42467.67847222222</v>
       </c>
       <c r="C27" s="1">
-        <v>42467.679861111108</v>
+        <v>42467.67986111111</v>
       </c>
       <c r="D27" s="1">
-        <v>42467.693749999999</v>
+        <v>42467.69375</v>
       </c>
       <c r="E27" s="1">
-        <v>42467.701388888891</v>
+        <v>42467.70138888889</v>
       </c>
       <c r="F27" s="1">
-        <v>42467.701388888891</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42467.70138888889</v>
+      </c>
+    </row>
+    <row r="28">
       <c r="A28" s="1">
         <v>42467.631944444445</v>
       </c>
       <c r="B28" s="1">
-        <v>42467.640277777777</v>
+        <v>42467.64027777778</v>
       </c>
       <c r="C28" s="1">
         <v>42467.64166666667</v>
@@ -964,18 +1003,18 @@
         <v>42467.660416666666</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>42467.106249999997</v>
+    <row r="29">
+      <c r="A29" s="3">
+        <v>42467.60625</v>
       </c>
       <c r="B29" s="1">
         <v>42467.611805555556</v>
       </c>
       <c r="C29" s="1">
-        <v>42467.613194444442</v>
+        <v>42467.61319444444</v>
       </c>
       <c r="D29" s="1">
-        <v>42467.619444444441</v>
+        <v>42467.61944444444</v>
       </c>
       <c r="E29" s="1">
         <v>42467.620833333334</v>
@@ -984,72 +1023,72 @@
         <v>42467.620833333334</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30">
       <c r="A30" s="1">
         <v>42467.583333333336</v>
       </c>
       <c r="B30" s="1">
-        <v>42467.588194444441</v>
+        <v>42467.58819444444</v>
       </c>
       <c r="C30" s="1">
-        <v>42467.590277777781</v>
+        <v>42467.59027777778</v>
       </c>
       <c r="D30" s="1">
-        <v>42467.593055555553</v>
+        <v>42467.59305555555</v>
       </c>
       <c r="E30" s="1">
-        <v>42467.595833333333</v>
+        <v>42467.59583333333</v>
       </c>
       <c r="F30" s="1">
-        <v>42467.595833333333</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42467.59583333333</v>
+      </c>
+    </row>
+    <row r="31">
       <c r="A31" s="1">
-        <v>42460.621527777781</v>
+        <v>42460.62152777778</v>
       </c>
       <c r="B31" s="1">
         <v>42460.631944444445</v>
       </c>
       <c r="C31" s="1">
-        <v>42460.634027777778</v>
+        <v>42460.63402777778</v>
       </c>
       <c r="D31" s="1">
-        <v>42460.645138888889</v>
+        <v>42460.64513888889</v>
       </c>
       <c r="E31" s="1">
-        <v>42460.655555555553</v>
+        <v>42460.65555555555</v>
       </c>
       <c r="F31" s="1">
-        <v>42460.655555555553</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42460.65555555555</v>
+      </c>
+    </row>
+    <row r="32">
       <c r="A32" s="1">
-        <v>42460.574999999997</v>
+        <v>42460.575</v>
       </c>
       <c r="B32" s="1">
-        <v>42460.582638888889</v>
+        <v>42460.58263888889</v>
       </c>
       <c r="C32" s="1">
-        <v>42460.585416666669</v>
+        <v>42460.58541666667</v>
       </c>
       <c r="D32" s="1">
         <v>42460.595138888886</v>
       </c>
       <c r="E32" s="1">
-        <v>42460.611111111109</v>
+        <v>42460.61111111111</v>
       </c>
       <c r="F32" s="1">
-        <v>42460.611111111109</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42460.61111111111</v>
+      </c>
+    </row>
+    <row r="33">
       <c r="A33" s="1">
         <v>42461.447916666664</v>
       </c>
       <c r="B33" s="1">
-        <v>42461.448611111111</v>
+        <v>42461.44861111111</v>
       </c>
       <c r="C33" s="1">
         <v>42461.447916666664</v>
@@ -1060,29 +1099,31 @@
       <c r="E33" s="1">
         <v>42461.475694444445</v>
       </c>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F33" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34">
       <c r="A34" s="1">
         <v>42460.45416666667</v>
       </c>
       <c r="B34" s="1">
-        <v>42460.459722222222</v>
+        <v>42460.45972222222</v>
       </c>
       <c r="C34" s="1">
-        <v>42460.463888888888</v>
+        <v>42460.46388888889</v>
       </c>
       <c r="D34" s="1">
-        <v>42460.481249999997</v>
+        <v>42460.48125</v>
       </c>
       <c r="E34" s="1">
-        <v>42460.488888888889</v>
+        <v>42460.48888888889</v>
       </c>
       <c r="F34" s="1">
         <v>42460.489583333336</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35">
       <c r="A35" s="1">
         <v>42464.436111111114</v>
       </c>
@@ -1090,39 +1131,39 @@
         <v>42464.447916666664</v>
       </c>
       <c r="C35" s="1">
-        <v>42464.451388888891</v>
+        <v>42464.45138888889</v>
       </c>
       <c r="D35" s="1">
-        <v>42464.616666666669</v>
-      </c>
-      <c r="E35" s="1">
-        <v>42464.131249999999</v>
+        <v>42464.61666666667</v>
+      </c>
+      <c r="E35" s="3">
+        <v>42464.63125</v>
       </c>
       <c r="F35" s="1">
         <v>42464.631944444445</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36">
       <c r="A36" s="1">
         <v>42464.379166666666</v>
       </c>
       <c r="B36" s="1">
-        <v>42464.387499999997</v>
+        <v>42464.3875</v>
       </c>
       <c r="C36" s="1">
-        <v>42464.388888888891</v>
+        <v>42464.38888888889</v>
       </c>
       <c r="D36" s="1">
         <v>42464.399305555555</v>
       </c>
       <c r="E36" s="1">
-        <v>42464.411111111112</v>
+        <v>42464.41111111111</v>
       </c>
       <c r="F36" s="1">
-        <v>42464.411111111112</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42464.41111111111</v>
+      </c>
+    </row>
+    <row r="37">
       <c r="A37" s="1">
         <v>42468.501388888886</v>
       </c>
@@ -1133,7 +1174,7 @@
         <v>42468.513194444444</v>
       </c>
       <c r="D37" s="1">
-        <v>42468.577777777777</v>
+        <v>42468.57777777778</v>
       </c>
       <c r="E37" s="1">
         <v>42468.59375</v>
@@ -1142,18 +1183,18 @@
         <v>42468.59375</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38">
       <c r="A38" s="1">
-        <v>42468.366666666669</v>
+        <v>42468.36666666667</v>
       </c>
       <c r="B38" s="1">
-        <v>42468.386805555558</v>
+        <v>42468.38680555556</v>
       </c>
       <c r="C38" s="1">
         <v>42468.396527777775</v>
       </c>
       <c r="D38" s="1">
-        <v>42468.477083333331</v>
+        <v>42468.47708333333</v>
       </c>
       <c r="E38" s="1">
         <v>42468.481944444444</v>
@@ -1162,7 +1203,7 @@
         <v>42468.481944444444</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39">
       <c r="A39" s="1">
         <v>42461.464583333334</v>
       </c>
@@ -1170,10 +1211,10 @@
         <v>42461.472916666666</v>
       </c>
       <c r="C39" s="1">
-        <v>42461.474999999999</v>
+        <v>42461.475</v>
       </c>
       <c r="D39" s="1">
-        <v>42461.482638888891</v>
+        <v>42461.48263888889</v>
       </c>
       <c r="E39" s="1">
         <v>42461.48541666667</v>
@@ -1182,33 +1223,35 @@
         <v>42461.48541666667</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40">
       <c r="A40" s="1">
-        <v>42461.392361111109</v>
+        <v>42461.39236111111</v>
       </c>
       <c r="B40" s="1">
         <v>42461.40625</v>
       </c>
       <c r="C40" s="1">
-        <v>42461.406944444447</v>
+        <v>42461.40694444445</v>
       </c>
       <c r="D40" s="1">
         <v>42461.415972222225</v>
       </c>
       <c r="E40" s="1">
-        <v>42461.440972222219</v>
+        <v>42461.44097222222</v>
       </c>
       <c r="F40" s="1">
-        <v>42461.443055555559</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
+        <v>42461.44305555556</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="B41" s="1">
-        <v>42447.643750000003</v>
+        <v>42447.64375</v>
       </c>
       <c r="C41" s="1">
-        <v>42447.648611111108</v>
+        <v>42447.64861111111</v>
       </c>
       <c r="D41" s="1">
         <v>42447.65347222222</v>
@@ -1217,35 +1260,35 @@
         <v>42447.654861111114</v>
       </c>
       <c r="F41" s="1">
-        <v>42447.654166666667</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42447.65416666667</v>
+      </c>
+    </row>
+    <row r="42">
       <c r="A42" s="1">
-        <v>42463.473611111112</v>
+        <v>42463.47361111111</v>
       </c>
       <c r="B42" s="1">
         <v>42463.479166666664</v>
       </c>
       <c r="C42" s="1">
-        <v>42463.486111111109</v>
+        <v>42463.48611111111</v>
       </c>
       <c r="D42" s="1">
-        <v>42463.513888888891</v>
+        <v>42463.51388888889</v>
       </c>
       <c r="E42" s="1">
         <v>42463.527083333334</v>
       </c>
       <c r="F42" s="1">
-        <v>42463.527777777781</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42463.52777777778</v>
+      </c>
+    </row>
+    <row r="43">
       <c r="A43" s="1">
         <v>42466.600694444445</v>
       </c>
       <c r="B43" s="1">
-        <v>42466.609722222223</v>
+        <v>42466.60972222222</v>
       </c>
       <c r="C43" s="1">
         <v>42466.611805555556</v>
@@ -1260,17 +1303,19 @@
         <v>42466.65625</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44">
       <c r="A44" s="1">
-        <v>42481.713194444441</v>
+        <v>42481.71319444444</v>
       </c>
       <c r="B44" s="1">
         <v>42481.71875</v>
       </c>
       <c r="C44" s="1">
-        <v>42481.722222222219</v>
-      </c>
-      <c r="D44" s="1"/>
+        <v>42481.72222222222</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E44" s="1">
         <v>42481.74722222222</v>
       </c>
@@ -1278,18 +1323,18 @@
         <v>42481.748611111114</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45">
       <c r="A45" s="1">
         <v>42481.666666666664</v>
       </c>
       <c r="B45" s="1">
-        <v>42481.684027777781</v>
+        <v>42481.68402777778</v>
       </c>
       <c r="C45" s="1">
         <v>42481.68472222222</v>
       </c>
       <c r="D45" s="1">
-        <v>42481.698611111111</v>
+        <v>42481.69861111111</v>
       </c>
       <c r="E45" s="1">
         <v>42481.70208333333</v>
@@ -1298,12 +1343,12 @@
         <v>42481.70416666667</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46">
       <c r="A46" s="1">
-        <v>42481.628472222219</v>
+        <v>42481.62847222222</v>
       </c>
       <c r="B46" s="1">
-        <v>42481.636805555558</v>
+        <v>42481.63680555556</v>
       </c>
       <c r="C46" s="1">
         <v>42481.638194444444</v>
@@ -1312,13 +1357,13 @@
         <v>42481.646527777775</v>
       </c>
       <c r="E46" s="1">
-        <v>42481.662499999999</v>
+        <v>42481.6625</v>
       </c>
       <c r="F46" s="1">
         <v>42481.663194444445</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47">
       <c r="A47" s="1">
         <v>42481.59375</v>
       </c>
@@ -1326,24 +1371,24 @@
         <v>42481.600694444445</v>
       </c>
       <c r="C47" s="1">
-        <v>42481.602083333331</v>
+        <v>42481.60208333333</v>
       </c>
       <c r="D47" s="1">
-        <v>42481.611111111109</v>
+        <v>42481.61111111111</v>
       </c>
       <c r="E47" s="1">
         <v>42481.623611111114</v>
       </c>
       <c r="F47" s="1">
-        <v>42481.624305555553</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42481.62430555555</v>
+      </c>
+    </row>
+    <row r="48">
       <c r="A48" s="1">
         <v>42481.572916666664</v>
       </c>
       <c r="B48" s="1">
-        <v>42481.577777777777</v>
+        <v>42481.57777777778</v>
       </c>
       <c r="C48" s="1">
         <v>42481.580555555556</v>
@@ -1351,94 +1396,96 @@
       <c r="D48" s="1">
         <v>42481.586805555555</v>
       </c>
-      <c r="E48" s="1"/>
+      <c r="E48" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F48" s="1">
         <v>42481.589583333334</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49">
       <c r="A49" s="1">
-        <v>42482.701388888891</v>
+        <v>42482.70138888889</v>
       </c>
       <c r="B49" s="1">
         <v>42482.711805555555</v>
       </c>
-      <c r="C49" s="1">
-        <v>42482.214583333334</v>
+      <c r="C49" s="3">
+        <v>42482.714583333334</v>
       </c>
       <c r="D49" s="1">
-        <v>42482.716666666667</v>
+        <v>42482.71666666667</v>
       </c>
       <c r="E49" s="1">
         <v>42482.71875</v>
       </c>
       <c r="F49" s="1">
-        <v>42482.719444444447</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42482.71944444445</v>
+      </c>
+    </row>
+    <row r="50">
       <c r="A50" s="1">
         <v>42482.67291666667</v>
       </c>
       <c r="B50" s="1">
-        <v>42482.681944444441</v>
+        <v>42482.68194444444</v>
       </c>
       <c r="C50" s="1">
         <v>42482.683333333334</v>
       </c>
       <c r="D50" s="1">
-        <v>42482.693749999999</v>
+        <v>42482.69375</v>
       </c>
       <c r="E50" s="1">
-        <v>42482.701388888891</v>
+        <v>42482.70138888889</v>
       </c>
       <c r="F50" s="1">
-        <v>42482.701388888891</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42482.70138888889</v>
+      </c>
+    </row>
+    <row r="51">
       <c r="A51" s="1">
-        <v>42482.638888888891</v>
+        <v>42482.63888888889</v>
       </c>
       <c r="B51" s="1">
         <v>42482.645833333336</v>
       </c>
       <c r="C51" s="1">
-        <v>42482.647222222222</v>
+        <v>42482.64722222222</v>
       </c>
       <c r="D51" s="1">
         <v>42482.654861111114</v>
       </c>
       <c r="E51" s="1">
-        <v>42482.655555555553</v>
+        <v>42482.65555555555</v>
       </c>
       <c r="F51" s="1">
         <v>42482.666666666664</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52">
       <c r="A52" s="1">
         <v>42496.63958333333</v>
       </c>
       <c r="B52" s="1">
-        <v>42496.648611111108</v>
+        <v>42496.64861111111</v>
       </c>
       <c r="C52" s="1">
         <v>42496.65</v>
       </c>
       <c r="D52" s="1">
-        <v>42496.668749999997</v>
+        <v>42496.66875</v>
       </c>
       <c r="E52" s="1">
-        <v>42496.673611111109</v>
+        <v>42496.67361111111</v>
       </c>
       <c r="F52" s="1">
-        <v>42496.673611111109</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42496.67361111111</v>
+      </c>
+    </row>
+    <row r="53">
       <c r="A53" s="1">
-        <v>42496.581250000003</v>
+        <v>42496.58125</v>
       </c>
       <c r="B53" s="1">
         <v>42496.59097222222</v>
@@ -1450,64 +1497,64 @@
         <v>42496.61041666667</v>
       </c>
       <c r="E53" s="1">
-        <v>42496.613194444442</v>
+        <v>42496.61319444444</v>
       </c>
       <c r="F53" s="1">
-        <v>42496.613194444442</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42496.61319444444</v>
+      </c>
+    </row>
+    <row r="54">
       <c r="A54" s="1">
         <v>42495.683333333334</v>
       </c>
       <c r="B54" s="1">
-        <v>42495.692361111112</v>
+        <v>42495.69236111111</v>
       </c>
       <c r="C54" s="1">
-        <v>42495.693055555559</v>
+        <v>42495.69305555556</v>
       </c>
       <c r="D54" s="1">
         <v>42495.70416666667</v>
       </c>
       <c r="E54" s="1">
-        <v>42495.712500000001</v>
+        <v>42495.7125</v>
       </c>
       <c r="F54" s="1">
-        <v>42495.718055555553</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42495.71805555555</v>
+      </c>
+    </row>
+    <row r="55">
       <c r="A55" s="1">
-        <v>42495.651388888888</v>
+        <v>42495.65138888889</v>
       </c>
       <c r="B55" s="1">
-        <v>42495.661111111112</v>
+        <v>42495.66111111111</v>
       </c>
       <c r="C55" s="1">
-        <v>42495.661805555559</v>
+        <v>42495.66180555556</v>
       </c>
       <c r="D55" s="1">
         <v>42495.669444444444</v>
       </c>
       <c r="E55" s="1">
-        <v>42495.679861111108</v>
+        <v>42495.67986111111</v>
       </c>
       <c r="F55" s="1">
-        <v>42495.679861111108</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42495.67986111111</v>
+      </c>
+    </row>
+    <row r="56">
       <c r="A56" s="1">
         <v>42495.618055555555</v>
       </c>
       <c r="B56" s="1">
-        <v>42495.627083333333</v>
+        <v>42495.62708333333</v>
       </c>
       <c r="C56" s="1">
         <v>42495.62777777778</v>
       </c>
       <c r="D56" s="1">
-        <v>42495.637499999997</v>
+        <v>42495.6375</v>
       </c>
       <c r="E56" s="1">
         <v>42495.649305555555</v>
@@ -1516,7 +1563,7 @@
         <v>42495.649305555555</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57">
       <c r="A57" s="1">
         <v>42495.592361111114</v>
       </c>
@@ -1530,33 +1577,33 @@
         <v>42495.606944444444</v>
       </c>
       <c r="E57" s="1">
-        <v>42495.612500000003</v>
+        <v>42495.6125</v>
       </c>
       <c r="F57" s="1">
-        <v>42495.612500000003</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42495.6125</v>
+      </c>
+    </row>
+    <row r="58">
       <c r="A58" s="1">
-        <v>42495.574305555558</v>
+        <v>42495.57430555556</v>
       </c>
       <c r="B58" s="1">
-        <v>42495.579861111109</v>
+        <v>42495.57986111111</v>
       </c>
       <c r="C58" s="1">
-        <v>42495.581250000003</v>
+        <v>42495.58125</v>
       </c>
       <c r="D58" s="1">
-        <v>42495.585416666669</v>
+        <v>42495.58541666667</v>
       </c>
       <c r="E58" s="1">
-        <v>42495.590277777781</v>
+        <v>42495.59027777778</v>
       </c>
       <c r="F58" s="1">
-        <v>42495.590277777781</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42495.59027777778</v>
+      </c>
+    </row>
+    <row r="59">
       <c r="A59" s="1">
         <v>42479.430555555555</v>
       </c>
@@ -1564,24 +1611,24 @@
         <v>42479.45</v>
       </c>
       <c r="C59" s="1">
-        <v>42479.453472222223</v>
+        <v>42479.45347222222</v>
       </c>
       <c r="D59" s="1">
-        <v>42479.465277777781</v>
+        <v>42479.46527777778</v>
       </c>
       <c r="E59" s="1">
-        <v>42479.477777777778</v>
+        <v>42479.47777777778</v>
       </c>
       <c r="F59" s="1">
-        <v>42479.477777777778</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42479.47777777778</v>
+      </c>
+    </row>
+    <row r="60">
       <c r="A60" s="1">
-        <v>42479.371527777781</v>
+        <v>42479.37152777778</v>
       </c>
       <c r="B60" s="1">
-        <v>42479.386111111111</v>
+        <v>42479.38611111111</v>
       </c>
       <c r="C60" s="1">
         <v>42479.388194444444</v>
@@ -1589,23 +1636,25 @@
       <c r="D60" s="1">
         <v>42479.404861111114</v>
       </c>
-      <c r="E60" s="1"/>
+      <c r="E60" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F60" s="1">
-        <v>42479.425694444442</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42479.42569444444</v>
+      </c>
+    </row>
+    <row r="61">
       <c r="A61" s="1">
-        <v>42489.647916666669</v>
+        <v>42489.64791666667</v>
       </c>
       <c r="B61" s="1">
-        <v>42489.652777777781</v>
+        <v>42489.65277777778</v>
       </c>
       <c r="C61" s="1">
-        <v>42489.654166666667</v>
+        <v>42489.65416666667</v>
       </c>
       <c r="D61" s="1">
-        <v>42489.659722222219</v>
+        <v>42489.65972222222</v>
       </c>
       <c r="E61" s="1">
         <v>42489.663194444445</v>
@@ -1614,47 +1663,47 @@
         <v>42489.663194444445</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62">
       <c r="A62" s="1">
         <v>42489.626388888886</v>
       </c>
       <c r="B62" s="1">
-        <v>42489.631249999999</v>
+        <v>42489.63125</v>
       </c>
       <c r="C62" s="1">
-        <v>42489.642361111109</v>
+        <v>42489.64236111111</v>
       </c>
       <c r="D62" s="1">
         <v>42489.64166666667</v>
       </c>
       <c r="E62" s="1">
-        <v>42489.642361111109</v>
+        <v>42489.64236111111</v>
       </c>
       <c r="F62" s="1">
-        <v>42489.642361111109</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42489.64236111111</v>
+      </c>
+    </row>
+    <row r="63">
       <c r="A63" s="1">
-        <v>42489.588194444441</v>
+        <v>42489.58819444444</v>
       </c>
       <c r="B63" s="1">
         <v>42489.59375</v>
       </c>
       <c r="C63" s="1">
-        <v>42489.597222222219</v>
+        <v>42489.59722222222</v>
       </c>
       <c r="D63" s="1">
-        <v>42489.611111111109</v>
+        <v>42489.61111111111</v>
       </c>
       <c r="E63" s="1">
-        <v>42489.622916666667</v>
+        <v>42489.62291666667</v>
       </c>
       <c r="F63" s="1">
         <v>42489.638194444444</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64">
       <c r="A64" s="1">
         <v>42474.486805555556</v>
       </c>
@@ -1665,21 +1714,21 @@
         <v>42474.495833333334</v>
       </c>
       <c r="D64" s="1">
-        <v>42474.507638888892</v>
+        <v>42474.50763888889</v>
       </c>
       <c r="E64" s="1">
-        <v>42474.520138888889</v>
+        <v>42474.52013888889</v>
       </c>
       <c r="F64" s="1">
         <v>42474.520833333336</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65">
       <c r="A65" s="1">
-        <v>42474.459722222222</v>
+        <v>42474.45972222222</v>
       </c>
       <c r="B65" s="1">
-        <v>42474.465277777781</v>
+        <v>42474.46527777778</v>
       </c>
       <c r="C65" s="1">
         <v>42474.46875</v>
@@ -1691,30 +1740,30 @@
         <v>42474.48333333333</v>
       </c>
       <c r="F65" s="1">
-        <v>42474.484027777777</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42474.48402777778</v>
+      </c>
+    </row>
+    <row r="66">
       <c r="A66" s="1">
         <v>42474.438888888886</v>
       </c>
       <c r="B66" s="1">
-        <v>42474.443749999999</v>
+        <v>42474.44375</v>
       </c>
       <c r="C66" s="1">
-        <v>42474.443749999999</v>
+        <v>42474.44375</v>
       </c>
       <c r="D66" s="1">
         <v>42474.45416666667</v>
       </c>
       <c r="E66" s="1">
-        <v>42474.454861111109</v>
+        <v>42474.45486111111</v>
       </c>
       <c r="F66" s="1">
         <v>42474.455555555556</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67">
       <c r="A67" s="1">
         <v>42474.415972222225</v>
       </c>
@@ -1728,7 +1777,7 @@
         <v>42474.424305555556</v>
       </c>
       <c r="E67" s="1">
-        <v>42474.429861111108</v>
+        <v>42474.42986111111</v>
       </c>
       <c r="F67" s="1">
         <v>42474.430555555555</v>
@@ -1736,6 +1785,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added functionality to handle one data being creater than the other when its not possible. Need to tidy code, and make it stronger and more flexible.
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -72,12 +72,17 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000" tint="0"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -107,11 +112,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1090,7 +1096,7 @@
       <c r="B33" s="1">
         <v>42461.44861111111</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="4">
         <v>42461.447916666664</v>
       </c>
       <c r="D33" s="1">
@@ -1259,7 +1265,7 @@
       <c r="E41" s="1">
         <v>42447.654861111114</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F41" s="4">
         <v>42447.65416666667</v>
       </c>
     </row>
@@ -1673,7 +1679,7 @@
       <c r="C62" s="1">
         <v>42489.64236111111</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D62" s="4">
         <v>42489.64166666667</v>
       </c>
       <c r="E62" s="1">

</xml_diff>

<commit_message>
Reformatted some code and added extra validation check in
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://medicorsoftware-my.sharepoint.com/personal/kris_medicorsoftware_com/Documents/Medicor/HR/Software dev Job Ad/Presentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Medicor\MedicorDataFormatter\OriginalDataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B6FCF0-02F7-441C-AE37-E6B4CDAA7766}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10808" xr2:uid="{1DB53C1C-FD47-4BB3-BB48-F7AD535890F0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1DB53C1C-FD47-4BB3-BB48-F7AD535890F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -85,7 +86,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -108,15 +109,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF0000FF" tint="0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF0000FF" tint="0"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF0000FF" tint="0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF0000FF" tint="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -433,20 +450,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8EA0C53-A141-40AA-B759-62088F3C5F05}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69:XFD69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="20.46484375" customWidth="1" style="2"/>
-    <col min="2" max="2" bestFit="1" width="14.53125" customWidth="1" style="2"/>
-    <col min="3" max="3" bestFit="1" width="14.9296875" customWidth="1" style="2"/>
-    <col min="4" max="4" bestFit="1" width="15.53125" customWidth="1" style="2"/>
-    <col min="5" max="5" bestFit="1" width="16.1328125" customWidth="1" style="2"/>
-    <col min="6" max="6" bestFit="1" width="15.86328125" customWidth="1" style="2"/>
+    <col min="1" max="1" bestFit="1" width="20.42578125" customWidth="1" style="2"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1" style="2"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1" style="2"/>
+    <col min="4" max="4" bestFit="1" width="15.5703125" customWidth="1" style="2"/>
+    <col min="5" max="5" bestFit="1" width="16.140625" customWidth="1" style="2"/>
+    <col min="6" max="6" bestFit="1" width="15.85546875" customWidth="1" style="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1096,7 +1113,7 @@
       <c r="B33" s="1">
         <v>42461.44861111111</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="5">
         <v>42461.447916666664</v>
       </c>
       <c r="D33" s="1">
@@ -1265,7 +1282,7 @@
       <c r="E41" s="1">
         <v>42447.654861111114</v>
       </c>
-      <c r="F41" s="4">
+      <c r="F41" s="5">
         <v>42447.65416666667</v>
       </c>
     </row>
@@ -1679,7 +1696,7 @@
       <c r="C62" s="1">
         <v>42489.64236111111</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D62" s="5">
         <v>42489.64166666667</v>
       </c>
       <c r="E62" s="1">
@@ -1787,6 +1804,26 @@
       </c>
       <c r="F67" s="1">
         <v>42474.430555555555</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="4">
+        <v>42474.875</v>
+      </c>
+      <c r="B68" s="3">
+        <v>42474.875</v>
+      </c>
+      <c r="C68" s="1">
+        <v>42474.895833333336</v>
+      </c>
+      <c r="D68" s="1">
+        <v>42474.895833333336</v>
+      </c>
+      <c r="E68" s="1">
+        <v>42474.895833333336</v>
+      </c>
+      <c r="F68" s="1">
+        <v>42474.895833333336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added dependency injection into console app. Added config file to make soluation more flexiable.
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -45,7 +45,7 @@
     <t>Time into Recovery</t>
   </si>
   <si>
-    <t>Time Out of Recovery</t>
+    <t>Time Out of Theatre</t>
   </si>
   <si>
     <t>Time of Anaesthetic Start</t>
@@ -64,10 +64,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,12 +93,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00BFFF" tint="0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00BFFF" tint="0"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF00BFFF" tint="0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00BFFF" tint="0"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -128,13 +150,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,7 +510,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -502,7 +525,7 @@
       <c r="E2" s="1">
         <v>42364.68680555555</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -550,7 +573,7 @@
       <c r="A5" s="1">
         <v>42671.52777777778</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>42671.56805555556</v>
       </c>
       <c r="C5" s="1">
@@ -559,7 +582,7 @@
       <c r="D5" s="1">
         <v>42671.63055555556</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>42671.64097222222</v>
       </c>
       <c r="F5" s="1">
@@ -567,7 +590,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>42670.59652777778</v>
       </c>
       <c r="B6" s="1">
@@ -642,7 +665,7 @@
       <c r="E9" s="1">
         <v>42408.29027777778</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -662,7 +685,7 @@
       <c r="E10" s="1">
         <v>42442.836805555555</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -707,7 +730,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1">
@@ -770,7 +793,7 @@
       <c r="A16" s="1">
         <v>42464.60208333333</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1">
@@ -779,7 +802,7 @@
       <c r="D16" s="1">
         <v>42464.666666666664</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="4">
         <v>42464.675</v>
       </c>
       <c r="F16" s="1">
@@ -882,7 +905,7 @@
       <c r="E21" s="1">
         <v>42468.6375</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="4">
         <v>42468.6375</v>
       </c>
     </row>
@@ -893,7 +916,7 @@
       <c r="B22" s="1">
         <v>42468.58888888889</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="1">
@@ -1027,7 +1050,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="3">
+      <c r="A29" s="4">
         <v>42467.60625</v>
       </c>
       <c r="B29" s="1">
@@ -1113,7 +1136,7 @@
       <c r="B33" s="1">
         <v>42461.44861111111</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="6">
         <v>42461.447916666664</v>
       </c>
       <c r="D33" s="1">
@@ -1122,7 +1145,7 @@
       <c r="E33" s="1">
         <v>42461.475694444445</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1159,7 +1182,7 @@
       <c r="D35" s="1">
         <v>42464.61666666667</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="4">
         <v>42464.63125</v>
       </c>
       <c r="F35" s="1">
@@ -1267,7 +1290,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="1">
@@ -1282,7 +1305,7 @@
       <c r="E41" s="1">
         <v>42447.654861111114</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="6">
         <v>42447.65416666667</v>
       </c>
     </row>
@@ -1336,7 +1359,7 @@
       <c r="C44" s="1">
         <v>42481.72222222222</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E44" s="1">
@@ -1419,7 +1442,7 @@
       <c r="D48" s="1">
         <v>42481.586805555555</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F48" s="1">
@@ -1433,7 +1456,7 @@
       <c r="B49" s="1">
         <v>42482.711805555555</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="4">
         <v>42482.714583333334</v>
       </c>
       <c r="D49" s="1">
@@ -1659,7 +1682,7 @@
       <c r="D60" s="1">
         <v>42479.404861111114</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F60" s="1">
@@ -1696,7 +1719,7 @@
       <c r="C62" s="1">
         <v>42489.64236111111</v>
       </c>
-      <c r="D62" s="5">
+      <c r="D62" s="6">
         <v>42489.64166666667</v>
       </c>
       <c r="E62" s="1">
@@ -1807,10 +1830,10 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="4">
+      <c r="A68" s="5">
         <v>42474.875</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B68" s="4">
         <v>42474.875</v>
       </c>
       <c r="C68" s="1">

</xml_diff>

<commit_message>
Added unit tests and refactored coded mroe
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Medicor\MedicorDataFormatter\OriginalDataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://medicorsoftware-my.sharepoint.com/personal/kris_medicorsoftware_com/Documents/Medicor/HR/Software dev Job Ad/Presentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B6FCF0-02F7-441C-AE37-E6B4CDAA7766}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1DB53C1C-FD47-4BB3-BB48-F7AD535890F0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10808" xr2:uid="{1DB53C1C-FD47-4BB3-BB48-F7AD535890F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -93,7 +92,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -131,32 +130,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF0000FF" tint="0"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF0000FF" tint="0"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF0000FF" tint="0"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF0000FF" tint="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -473,20 +456,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8EA0C53-A141-40AA-B759-62088F3C5F05}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:XFD69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="20.42578125" customWidth="1" style="2"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1" style="2"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1" style="2"/>
-    <col min="4" max="4" bestFit="1" width="15.5703125" customWidth="1" style="2"/>
-    <col min="5" max="5" bestFit="1" width="16.140625" customWidth="1" style="2"/>
-    <col min="6" max="6" bestFit="1" width="15.85546875" customWidth="1" style="2"/>
+    <col min="1" max="1" bestFit="1" width="20.46484375" customWidth="1" style="2"/>
+    <col min="2" max="2" bestFit="1" width="14.53125" customWidth="1" style="2"/>
+    <col min="3" max="3" bestFit="1" width="14.9296875" customWidth="1" style="2"/>
+    <col min="4" max="4" bestFit="1" width="15.53125" customWidth="1" style="2"/>
+    <col min="5" max="5" bestFit="1" width="16.1328125" customWidth="1" style="2"/>
+    <col min="6" max="6" bestFit="1" width="15.86328125" customWidth="1" style="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1136,7 +1119,7 @@
       <c r="B33" s="1">
         <v>42461.44861111111</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="5">
         <v>42461.447916666664</v>
       </c>
       <c r="D33" s="1">
@@ -1305,7 +1288,7 @@
       <c r="E41" s="1">
         <v>42447.654861111114</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F41" s="5">
         <v>42447.65416666667</v>
       </c>
     </row>
@@ -1719,7 +1702,7 @@
       <c r="C62" s="1">
         <v>42489.64236111111</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D62" s="1">
         <v>42489.64166666667</v>
       </c>
       <c r="E62" s="1">
@@ -1827,26 +1810,6 @@
       </c>
       <c r="F67" s="1">
         <v>42474.430555555555</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="5">
-        <v>42474.875</v>
-      </c>
-      <c r="B68" s="4">
-        <v>42474.875</v>
-      </c>
-      <c r="C68" s="1">
-        <v>42474.895833333336</v>
-      </c>
-      <c r="D68" s="1">
-        <v>42474.895833333336</v>
-      </c>
-      <c r="E68" s="1">
-        <v>42474.895833333336</v>
-      </c>
-      <c r="F68" s="1">
-        <v>42474.895833333336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made code more readable in formatter class
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Time of anaesthetic start</t>
   </si>
@@ -43,6 +43,18 @@
   <si>
     <t>Time into Recovery</t>
   </si>
+  <si>
+    <t>Time Out of Theatre</t>
+  </si>
+  <si>
+    <t>Time of Anaesthetic Start</t>
+  </si>
+  <si>
+    <t>Time into Theatre</t>
+  </si>
+  <si>
+    <t>Time out of Theatre</t>
+  </si>
 </sst>
 </file>
 
@@ -51,7 +63,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,16 +71,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000" tint="0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -76,14 +100,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00BFFF" tint="0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00BFFF" tint="0"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF00BFFF" tint="0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00BFFF" tint="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000" tint="0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFF0000" tint="0"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000" tint="0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000" tint="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,15 +464,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.46484375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.53125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.9296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.53125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="20.46484375" customWidth="1" style="2"/>
+    <col min="2" max="2" bestFit="1" width="14.53125" customWidth="1" style="2"/>
+    <col min="3" max="3" bestFit="1" width="14.9296875" customWidth="1" style="2"/>
+    <col min="4" max="4" bestFit="1" width="15.53125" customWidth="1" style="2"/>
+    <col min="5" max="5" bestFit="1" width="16.1328125" customWidth="1" style="2"/>
+    <col min="6" max="6" bestFit="1" width="15.86328125" customWidth="1" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,25 +492,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="1"/>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="B2" s="1">
-        <v>42364.648611111108</v>
+        <v>42364.64861111111</v>
       </c>
       <c r="C2" s="1">
-        <v>42364.661805555559</v>
+        <v>42364.66180555556</v>
       </c>
       <c r="D2" s="1">
-        <v>42364.675694444442</v>
+        <v>42364.67569444444</v>
       </c>
       <c r="E2" s="1">
-        <v>42364.686805555553</v>
-      </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42364.68680555555</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="1">
-        <v>42586.486111111109</v>
+        <v>42586.48611111111</v>
       </c>
       <c r="B3" s="1">
         <v>42586.5</v>
@@ -462,58 +523,58 @@
         <v>42586.5</v>
       </c>
       <c r="D3" s="1">
-        <v>42586.517361111109</v>
+        <v>42586.51736111111</v>
       </c>
       <c r="E3" s="1">
-        <v>42586.518750000003</v>
+        <v>42586.51875</v>
       </c>
       <c r="F3" s="1">
-        <v>42586.518750000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42586.51875</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="1">
         <v>42557.413194444445</v>
       </c>
       <c r="B4" s="1">
-        <v>42557.418749999997</v>
+        <v>42557.41875</v>
       </c>
       <c r="C4" s="1">
-        <v>42557.422222222223</v>
+        <v>42557.42222222222</v>
       </c>
       <c r="D4" s="1">
         <v>42557.436111111114</v>
       </c>
       <c r="E4" s="1">
-        <v>42557.443055555559</v>
+        <v>42557.44305555556</v>
       </c>
       <c r="F4" s="1">
-        <v>42557.443749999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42557.44375</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="1">
-        <v>42671.527777777781</v>
-      </c>
-      <c r="B5" s="1">
-        <v>42671.068055555559</v>
+        <v>42671.52777777778</v>
+      </c>
+      <c r="B5" s="4">
+        <v>42671.56805555556</v>
       </c>
       <c r="C5" s="1">
-        <v>42671.571527777778</v>
+        <v>42671.57152777778</v>
       </c>
       <c r="D5" s="1">
-        <v>42671.630555555559</v>
-      </c>
-      <c r="E5" s="1">
-        <v>42671.140972222223</v>
+        <v>42671.63055555556</v>
+      </c>
+      <c r="E5" s="4">
+        <v>42671.64097222222</v>
       </c>
       <c r="F5" s="1">
-        <v>42671.642361111109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
-        <v>42670.09652777778</v>
+        <v>42671.64236111111</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4">
+        <v>42670.59652777778</v>
       </c>
       <c r="B6" s="1">
         <v>42670.606944444444</v>
@@ -525,24 +586,24 @@
         <v>42670.634722222225</v>
       </c>
       <c r="E6" s="1">
-        <v>42670.652777777781</v>
+        <v>42670.65277777778</v>
       </c>
       <c r="F6" s="1">
         <v>42670.654861111114</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7">
       <c r="A7" s="1">
-        <v>42720.442361111112</v>
+        <v>42720.44236111111</v>
       </c>
       <c r="B7" s="1">
-        <v>42720.454861111109</v>
+        <v>42720.45486111111</v>
       </c>
       <c r="C7" s="1">
         <v>42720.458333333336</v>
       </c>
       <c r="D7" s="1">
-        <v>42720.522916666669</v>
+        <v>42720.52291666667</v>
       </c>
       <c r="E7" s="1">
         <v>42720.532638888886</v>
@@ -551,88 +612,92 @@
         <v>42720.53402777778</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8">
       <c r="A8" s="1">
-        <v>42405.518750000003</v>
+        <v>42405.51875</v>
       </c>
       <c r="B8" s="1">
-        <v>42405.519444444442</v>
+        <v>42405.51944444444</v>
       </c>
       <c r="C8" s="1">
-        <v>42405.520138888889</v>
+        <v>42405.52013888889</v>
       </c>
       <c r="D8" s="1">
-        <v>42405.533333333333</v>
+        <v>42405.53333333333</v>
       </c>
       <c r="E8" s="1">
-        <v>42405.550694444442</v>
+        <v>42405.55069444444</v>
       </c>
       <c r="F8" s="1">
         <v>42405.552777777775</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9">
       <c r="A9" s="1">
         <v>42408.21597222222</v>
       </c>
       <c r="B9" s="1">
-        <v>42408.216666666667</v>
+        <v>42408.21666666667</v>
       </c>
       <c r="C9" s="1">
-        <v>42408.230555555558</v>
+        <v>42408.23055555556</v>
       </c>
       <c r="D9" s="1">
-        <v>42408.267361111109</v>
+        <v>42408.26736111111</v>
       </c>
       <c r="E9" s="1">
-        <v>42408.290277777778</v>
-      </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42408.29027777778</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" s="1">
-        <v>42442.722222222219</v>
+        <v>42442.72222222222</v>
       </c>
       <c r="B10" s="1">
-        <v>42442.752083333333</v>
+        <v>42442.75208333333</v>
       </c>
       <c r="C10" s="1">
-        <v>42442.755555555559</v>
+        <v>42442.75555555556</v>
       </c>
       <c r="D10" s="1">
-        <v>42442.790277777778</v>
+        <v>42442.79027777778</v>
       </c>
       <c r="E10" s="1">
         <v>42442.836805555555</v>
       </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" s="1">
-        <v>42464.434027777781</v>
+        <v>42464.43402777778</v>
       </c>
       <c r="B11" s="1">
         <v>42464.436111111114</v>
       </c>
       <c r="C11" s="1">
-        <v>42464.438194444447</v>
+        <v>42464.43819444445</v>
       </c>
       <c r="D11" s="1">
         <v>42464.447916666664</v>
       </c>
       <c r="E11" s="1">
-        <v>42464.459722222222</v>
+        <v>42464.45972222222</v>
       </c>
       <c r="F11" s="1">
-        <v>42464.459722222222</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42464.45972222222</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" s="1">
         <v>42464.399305555555</v>
       </c>
       <c r="B12" s="1">
-        <v>42464.405555555553</v>
+        <v>42464.40555555555</v>
       </c>
       <c r="C12" s="1">
         <v>42464.40625</v>
@@ -641,14 +706,16 @@
         <v>42464.415972222225</v>
       </c>
       <c r="E12" s="1">
-        <v>42464.422222222223</v>
+        <v>42464.42222222222</v>
       </c>
       <c r="F12" s="1">
-        <v>42464.422222222223</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="1"/>
+        <v>42464.42222222222</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="B13" s="1">
         <v>42464.381944444445</v>
       </c>
@@ -656,16 +723,16 @@
         <v>42464.381944444445</v>
       </c>
       <c r="D13" s="1">
-        <v>42464.382638888892</v>
+        <v>42464.38263888889</v>
       </c>
       <c r="E13" s="1">
-        <v>42464.382638888892</v>
+        <v>42464.38263888889</v>
       </c>
       <c r="F13" s="1">
         <v>42464.388194444444</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14">
       <c r="A14" s="1">
         <v>42461.427083333336</v>
       </c>
@@ -676,7 +743,7 @@
         <v>42461.444444444445</v>
       </c>
       <c r="D14" s="1">
-        <v>42461.490972222222</v>
+        <v>42461.49097222222</v>
       </c>
       <c r="E14" s="1">
         <v>42461.5</v>
@@ -685,7 +752,7 @@
         <v>42461.501388888886</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15">
       <c r="A15" s="1">
         <v>42461.35833333333</v>
       </c>
@@ -696,36 +763,38 @@
         <v>42461.370833333334</v>
       </c>
       <c r="D15" s="1">
-        <v>42461.411805555559</v>
+        <v>42461.41180555556</v>
       </c>
       <c r="E15" s="1">
-        <v>42461.421527777777</v>
+        <v>42461.42152777778</v>
       </c>
       <c r="F15" s="1">
-        <v>42461.425000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42461.425</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" s="1">
-        <v>42464.602083333331</v>
-      </c>
-      <c r="B16" s="1"/>
+        <v>42464.60208333333</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="C16" s="1">
-        <v>42464.612500000003</v>
+        <v>42464.6125</v>
       </c>
       <c r="D16" s="1">
         <v>42464.666666666664</v>
       </c>
-      <c r="E16" s="1">
-        <v>42464.175000000003</v>
+      <c r="E16" s="4">
+        <v>42464.675</v>
       </c>
       <c r="F16" s="1">
-        <v>42464.675000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42464.675</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" s="1">
-        <v>42464.559027777781</v>
+        <v>42464.55902777778</v>
       </c>
       <c r="B17" s="1">
         <v>42464.5625</v>
@@ -737,58 +806,58 @@
         <v>42464.592361111114</v>
       </c>
       <c r="E17" s="1">
-        <v>42464.601388888892</v>
+        <v>42464.60138888889</v>
       </c>
       <c r="F17" s="1">
-        <v>42464.601388888892</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42464.60138888889</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18" s="1">
-        <v>42464.443055555559</v>
+        <v>42464.44305555556</v>
       </c>
       <c r="B18" s="1">
-        <v>42464.448611111111</v>
+        <v>42464.44861111111</v>
       </c>
       <c r="C18" s="1">
-        <v>42464.456944444442</v>
+        <v>42464.45694444444</v>
       </c>
       <c r="D18" s="1">
-        <v>42464.505555555559</v>
+        <v>42464.50555555556</v>
       </c>
       <c r="E18" s="1">
         <v>42464.513194444444</v>
       </c>
       <c r="F18" s="1">
-        <v>42464.513888888891</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42464.51388888889</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" s="1">
-        <v>42464.372916666667</v>
+        <v>42464.37291666667</v>
       </c>
       <c r="B19" s="1">
-        <v>42464.381249999999</v>
+        <v>42464.38125</v>
       </c>
       <c r="C19" s="1">
-        <v>42464.386111111111</v>
+        <v>42464.38611111111</v>
       </c>
       <c r="D19" s="1">
         <v>42464.436111111114</v>
       </c>
       <c r="E19" s="1">
-        <v>42464.438194444447</v>
+        <v>42464.43819444445</v>
       </c>
       <c r="F19" s="1">
-        <v>42464.439583333333</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42464.43958333333</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20" s="1">
         <v>42468.649305555555</v>
       </c>
       <c r="B20" s="1">
-        <v>42468.654166666667</v>
+        <v>42468.65416666667</v>
       </c>
       <c r="C20" s="1">
         <v>42468.65625</v>
@@ -803,7 +872,7 @@
         <v>42468.663194444445</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21">
       <c r="A21" s="1">
         <v>42468.615277777775</v>
       </c>
@@ -811,37 +880,39 @@
         <v>42468.629166666666</v>
       </c>
       <c r="C21" s="1">
-        <v>42468.629861111112</v>
+        <v>42468.62986111111</v>
       </c>
       <c r="D21" s="1">
         <v>42468.631944444445</v>
       </c>
       <c r="E21" s="1">
-        <v>42468.637499999997</v>
-      </c>
-      <c r="F21" s="1">
-        <v>42468.137499999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42468.6375</v>
+      </c>
+      <c r="F21" s="4">
+        <v>42468.6375</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" s="1">
         <v>42468.57708333333</v>
       </c>
       <c r="B22" s="1">
-        <v>42468.588888888888</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>42468.58888888889</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="D22" s="1">
-        <v>42468.602083333331</v>
+        <v>42468.60208333333</v>
       </c>
       <c r="E22" s="1">
-        <v>42468.611111111109</v>
+        <v>42468.61111111111</v>
       </c>
       <c r="F22" s="1">
-        <v>42468.611111111109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42468.61111111111</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" s="1">
         <v>42467.472916666666</v>
       </c>
@@ -855,24 +926,24 @@
         <v>42467.501388888886</v>
       </c>
       <c r="E23" s="1">
-        <v>42467.503472222219</v>
+        <v>42467.50347222222</v>
       </c>
       <c r="F23" s="1">
-        <v>42467.504861111112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42467.50486111111</v>
+      </c>
+    </row>
+    <row r="24">
       <c r="A24" s="1">
         <v>42467.455555555556</v>
       </c>
       <c r="B24" s="1">
-        <v>42467.456250000003</v>
+        <v>42467.45625</v>
       </c>
       <c r="C24" s="1">
-        <v>42467.456944444442</v>
+        <v>42467.45694444444</v>
       </c>
       <c r="D24" s="1">
-        <v>42467.461111111108</v>
+        <v>42467.46111111111</v>
       </c>
       <c r="E24" s="1">
         <v>42467.464583333334</v>
@@ -881,29 +952,29 @@
         <v>42467.464583333334</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25">
       <c r="A25" s="1">
         <v>42467.424305555556</v>
       </c>
       <c r="B25" s="1">
-        <v>42467.431250000001</v>
+        <v>42467.43125</v>
       </c>
       <c r="C25" s="1">
-        <v>42467.434027777781</v>
+        <v>42467.43402777778</v>
       </c>
       <c r="D25" s="1">
-        <v>42467.445138888892</v>
+        <v>42467.44513888889</v>
       </c>
       <c r="E25" s="1">
-        <v>42467.448611111111</v>
+        <v>42467.44861111111</v>
       </c>
       <c r="F25" s="1">
-        <v>42467.448611111111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42467.44861111111</v>
+      </c>
+    </row>
+    <row r="26">
       <c r="A26" s="1">
-        <v>42467.397222222222</v>
+        <v>42467.39722222222</v>
       </c>
       <c r="B26" s="1">
         <v>42467.40347222222</v>
@@ -915,38 +986,38 @@
         <v>42467.415972222225</v>
       </c>
       <c r="E26" s="1">
-        <v>42467.418749999997</v>
+        <v>42467.41875</v>
       </c>
       <c r="F26" s="1">
         <v>42467.419444444444</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27">
       <c r="A27" s="1">
-        <v>42467.673611111109</v>
+        <v>42467.67361111111</v>
       </c>
       <c r="B27" s="1">
-        <v>42467.678472222222</v>
+        <v>42467.67847222222</v>
       </c>
       <c r="C27" s="1">
-        <v>42467.679861111108</v>
+        <v>42467.67986111111</v>
       </c>
       <c r="D27" s="1">
-        <v>42467.693749999999</v>
+        <v>42467.69375</v>
       </c>
       <c r="E27" s="1">
-        <v>42467.701388888891</v>
+        <v>42467.70138888889</v>
       </c>
       <c r="F27" s="1">
-        <v>42467.701388888891</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42467.70138888889</v>
+      </c>
+    </row>
+    <row r="28">
       <c r="A28" s="1">
         <v>42467.631944444445</v>
       </c>
       <c r="B28" s="1">
-        <v>42467.640277777777</v>
+        <v>42467.64027777778</v>
       </c>
       <c r="C28" s="1">
         <v>42467.64166666667</v>
@@ -961,18 +1032,18 @@
         <v>42467.660416666666</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="1">
-        <v>42467.106249999997</v>
+    <row r="29">
+      <c r="A29" s="4">
+        <v>42467.60625</v>
       </c>
       <c r="B29" s="1">
         <v>42467.611805555556</v>
       </c>
       <c r="C29" s="1">
-        <v>42467.613194444442</v>
+        <v>42467.61319444444</v>
       </c>
       <c r="D29" s="1">
-        <v>42467.619444444441</v>
+        <v>42467.61944444444</v>
       </c>
       <c r="E29" s="1">
         <v>42467.620833333334</v>
@@ -981,74 +1052,74 @@
         <v>42467.620833333334</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30">
       <c r="A30" s="1">
         <v>42467.583333333336</v>
       </c>
       <c r="B30" s="1">
-        <v>42467.588194444441</v>
+        <v>42467.58819444444</v>
       </c>
       <c r="C30" s="1">
-        <v>42467.590277777781</v>
+        <v>42467.59027777778</v>
       </c>
       <c r="D30" s="1">
-        <v>42467.593055555553</v>
+        <v>42467.59305555555</v>
       </c>
       <c r="E30" s="1">
-        <v>42467.595833333333</v>
+        <v>42467.59583333333</v>
       </c>
       <c r="F30" s="1">
-        <v>42467.595833333333</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42467.59583333333</v>
+      </c>
+    </row>
+    <row r="31">
       <c r="A31" s="1">
-        <v>42460.621527777781</v>
+        <v>42460.62152777778</v>
       </c>
       <c r="B31" s="1">
         <v>42460.631944444445</v>
       </c>
       <c r="C31" s="1">
-        <v>42460.634027777778</v>
+        <v>42460.63402777778</v>
       </c>
       <c r="D31" s="1">
-        <v>42460.645138888889</v>
+        <v>42460.64513888889</v>
       </c>
       <c r="E31" s="1">
-        <v>42460.655555555553</v>
+        <v>42460.65555555555</v>
       </c>
       <c r="F31" s="1">
-        <v>42460.655555555553</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42460.65555555555</v>
+      </c>
+    </row>
+    <row r="32">
       <c r="A32" s="1">
-        <v>42460.574999999997</v>
+        <v>42460.575</v>
       </c>
       <c r="B32" s="1">
-        <v>42460.582638888889</v>
+        <v>42460.58263888889</v>
       </c>
       <c r="C32" s="1">
-        <v>42460.585416666669</v>
+        <v>42460.58541666667</v>
       </c>
       <c r="D32" s="1">
         <v>42460.595138888886</v>
       </c>
       <c r="E32" s="1">
-        <v>42460.611111111109</v>
+        <v>42460.61111111111</v>
       </c>
       <c r="F32" s="1">
-        <v>42460.611111111109</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42460.61111111111</v>
+      </c>
+    </row>
+    <row r="33">
       <c r="A33" s="1">
         <v>42461.447916666664</v>
       </c>
       <c r="B33" s="1">
-        <v>42461.448611111111</v>
-      </c>
-      <c r="C33" s="1">
+        <v>42461.44861111111</v>
+      </c>
+      <c r="C33" s="5">
         <v>42461.447916666664</v>
       </c>
       <c r="D33" s="1">
@@ -1057,29 +1128,31 @@
       <c r="E33" s="1">
         <v>42461.475694444445</v>
       </c>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F33" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34">
       <c r="A34" s="1">
         <v>42460.45416666667</v>
       </c>
       <c r="B34" s="1">
-        <v>42460.459722222222</v>
+        <v>42460.45972222222</v>
       </c>
       <c r="C34" s="1">
-        <v>42460.463888888888</v>
+        <v>42460.46388888889</v>
       </c>
       <c r="D34" s="1">
-        <v>42460.481249999997</v>
+        <v>42460.48125</v>
       </c>
       <c r="E34" s="1">
-        <v>42460.488888888889</v>
+        <v>42460.48888888889</v>
       </c>
       <c r="F34" s="1">
         <v>42460.489583333336</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35">
       <c r="A35" s="1">
         <v>42464.436111111114</v>
       </c>
@@ -1087,39 +1160,39 @@
         <v>42464.447916666664</v>
       </c>
       <c r="C35" s="1">
-        <v>42464.451388888891</v>
+        <v>42464.45138888889</v>
       </c>
       <c r="D35" s="1">
-        <v>42464.616666666669</v>
-      </c>
-      <c r="E35" s="1">
-        <v>42464.131249999999</v>
+        <v>42464.61666666667</v>
+      </c>
+      <c r="E35" s="4">
+        <v>42464.63125</v>
       </c>
       <c r="F35" s="1">
         <v>42464.631944444445</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36">
       <c r="A36" s="1">
         <v>42464.379166666666</v>
       </c>
       <c r="B36" s="1">
-        <v>42464.387499999997</v>
+        <v>42464.3875</v>
       </c>
       <c r="C36" s="1">
-        <v>42464.388888888891</v>
+        <v>42464.38888888889</v>
       </c>
       <c r="D36" s="1">
         <v>42464.399305555555</v>
       </c>
       <c r="E36" s="1">
-        <v>42464.411111111112</v>
+        <v>42464.41111111111</v>
       </c>
       <c r="F36" s="1">
-        <v>42464.411111111112</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42464.41111111111</v>
+      </c>
+    </row>
+    <row r="37">
       <c r="A37" s="1">
         <v>42468.501388888886</v>
       </c>
@@ -1130,7 +1203,7 @@
         <v>42468.513194444444</v>
       </c>
       <c r="D37" s="1">
-        <v>42468.577777777777</v>
+        <v>42468.57777777778</v>
       </c>
       <c r="E37" s="1">
         <v>42468.59375</v>
@@ -1139,18 +1212,18 @@
         <v>42468.59375</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38">
       <c r="A38" s="1">
-        <v>42468.366666666669</v>
+        <v>42468.36666666667</v>
       </c>
       <c r="B38" s="1">
-        <v>42468.386805555558</v>
+        <v>42468.38680555556</v>
       </c>
       <c r="C38" s="1">
         <v>42468.396527777775</v>
       </c>
       <c r="D38" s="1">
-        <v>42468.477083333331</v>
+        <v>42468.47708333333</v>
       </c>
       <c r="E38" s="1">
         <v>42468.481944444444</v>
@@ -1159,7 +1232,7 @@
         <v>42468.481944444444</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39">
       <c r="A39" s="1">
         <v>42461.464583333334</v>
       </c>
@@ -1167,10 +1240,10 @@
         <v>42461.472916666666</v>
       </c>
       <c r="C39" s="1">
-        <v>42461.474999999999</v>
+        <v>42461.475</v>
       </c>
       <c r="D39" s="1">
-        <v>42461.482638888891</v>
+        <v>42461.48263888889</v>
       </c>
       <c r="E39" s="1">
         <v>42461.48541666667</v>
@@ -1179,33 +1252,35 @@
         <v>42461.48541666667</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40">
       <c r="A40" s="1">
-        <v>42461.392361111109</v>
+        <v>42461.39236111111</v>
       </c>
       <c r="B40" s="1">
         <v>42461.40625</v>
       </c>
       <c r="C40" s="1">
-        <v>42461.406944444447</v>
+        <v>42461.40694444445</v>
       </c>
       <c r="D40" s="1">
         <v>42461.415972222225</v>
       </c>
       <c r="E40" s="1">
-        <v>42461.440972222219</v>
+        <v>42461.44097222222</v>
       </c>
       <c r="F40" s="1">
-        <v>42461.443055555559</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="1"/>
+        <v>42461.44305555556</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="B41" s="1">
-        <v>42447.643750000003</v>
+        <v>42447.64375</v>
       </c>
       <c r="C41" s="1">
-        <v>42447.648611111108</v>
+        <v>42447.64861111111</v>
       </c>
       <c r="D41" s="1">
         <v>42447.65347222222</v>
@@ -1213,36 +1288,36 @@
       <c r="E41" s="1">
         <v>42447.654861111114</v>
       </c>
-      <c r="F41" s="1">
-        <v>42447.654166666667</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F41" s="5">
+        <v>42447.65416666667</v>
+      </c>
+    </row>
+    <row r="42">
       <c r="A42" s="1">
-        <v>42463.473611111112</v>
+        <v>42463.47361111111</v>
       </c>
       <c r="B42" s="1">
         <v>42463.479166666664</v>
       </c>
       <c r="C42" s="1">
-        <v>42463.486111111109</v>
+        <v>42463.48611111111</v>
       </c>
       <c r="D42" s="1">
-        <v>42463.513888888891</v>
+        <v>42463.51388888889</v>
       </c>
       <c r="E42" s="1">
         <v>42463.527083333334</v>
       </c>
       <c r="F42" s="1">
-        <v>42463.527777777781</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42463.52777777778</v>
+      </c>
+    </row>
+    <row r="43">
       <c r="A43" s="1">
         <v>42466.600694444445</v>
       </c>
       <c r="B43" s="1">
-        <v>42466.609722222223</v>
+        <v>42466.60972222222</v>
       </c>
       <c r="C43" s="1">
         <v>42466.611805555556</v>
@@ -1257,17 +1332,19 @@
         <v>42466.65625</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44">
       <c r="A44" s="1">
-        <v>42481.713194444441</v>
+        <v>42481.71319444444</v>
       </c>
       <c r="B44" s="1">
         <v>42481.71875</v>
       </c>
       <c r="C44" s="1">
-        <v>42481.722222222219</v>
-      </c>
-      <c r="D44" s="1"/>
+        <v>42481.72222222222</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="E44" s="1">
         <v>42481.74722222222</v>
       </c>
@@ -1275,18 +1352,18 @@
         <v>42481.748611111114</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45">
       <c r="A45" s="1">
         <v>42481.666666666664</v>
       </c>
       <c r="B45" s="1">
-        <v>42481.684027777781</v>
+        <v>42481.68402777778</v>
       </c>
       <c r="C45" s="1">
         <v>42481.68472222222</v>
       </c>
       <c r="D45" s="1">
-        <v>42481.698611111111</v>
+        <v>42481.69861111111</v>
       </c>
       <c r="E45" s="1">
         <v>42481.70208333333</v>
@@ -1295,12 +1372,12 @@
         <v>42481.70416666667</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46">
       <c r="A46" s="1">
-        <v>42481.628472222219</v>
+        <v>42481.62847222222</v>
       </c>
       <c r="B46" s="1">
-        <v>42481.636805555558</v>
+        <v>42481.63680555556</v>
       </c>
       <c r="C46" s="1">
         <v>42481.638194444444</v>
@@ -1309,13 +1386,13 @@
         <v>42481.646527777775</v>
       </c>
       <c r="E46" s="1">
-        <v>42481.662499999999</v>
+        <v>42481.6625</v>
       </c>
       <c r="F46" s="1">
         <v>42481.663194444445</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47">
       <c r="A47" s="1">
         <v>42481.59375</v>
       </c>
@@ -1323,24 +1400,24 @@
         <v>42481.600694444445</v>
       </c>
       <c r="C47" s="1">
-        <v>42481.602083333331</v>
+        <v>42481.60208333333</v>
       </c>
       <c r="D47" s="1">
-        <v>42481.611111111109</v>
+        <v>42481.61111111111</v>
       </c>
       <c r="E47" s="1">
         <v>42481.623611111114</v>
       </c>
       <c r="F47" s="1">
-        <v>42481.624305555553</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42481.62430555555</v>
+      </c>
+    </row>
+    <row r="48">
       <c r="A48" s="1">
         <v>42481.572916666664</v>
       </c>
       <c r="B48" s="1">
-        <v>42481.577777777777</v>
+        <v>42481.57777777778</v>
       </c>
       <c r="C48" s="1">
         <v>42481.580555555556</v>
@@ -1348,94 +1425,96 @@
       <c r="D48" s="1">
         <v>42481.586805555555</v>
       </c>
-      <c r="E48" s="1"/>
+      <c r="E48" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="F48" s="1">
         <v>42481.589583333334</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49">
       <c r="A49" s="1">
-        <v>42482.701388888891</v>
+        <v>42482.70138888889</v>
       </c>
       <c r="B49" s="1">
         <v>42482.711805555555</v>
       </c>
-      <c r="C49" s="1">
-        <v>42482.214583333334</v>
+      <c r="C49" s="4">
+        <v>42482.714583333334</v>
       </c>
       <c r="D49" s="1">
-        <v>42482.716666666667</v>
+        <v>42482.71666666667</v>
       </c>
       <c r="E49" s="1">
         <v>42482.71875</v>
       </c>
       <c r="F49" s="1">
-        <v>42482.719444444447</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42482.71944444445</v>
+      </c>
+    </row>
+    <row r="50">
       <c r="A50" s="1">
         <v>42482.67291666667</v>
       </c>
       <c r="B50" s="1">
-        <v>42482.681944444441</v>
+        <v>42482.68194444444</v>
       </c>
       <c r="C50" s="1">
         <v>42482.683333333334</v>
       </c>
       <c r="D50" s="1">
-        <v>42482.693749999999</v>
+        <v>42482.69375</v>
       </c>
       <c r="E50" s="1">
-        <v>42482.701388888891</v>
+        <v>42482.70138888889</v>
       </c>
       <c r="F50" s="1">
-        <v>42482.701388888891</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42482.70138888889</v>
+      </c>
+    </row>
+    <row r="51">
       <c r="A51" s="1">
-        <v>42482.638888888891</v>
+        <v>42482.63888888889</v>
       </c>
       <c r="B51" s="1">
         <v>42482.645833333336</v>
       </c>
       <c r="C51" s="1">
-        <v>42482.647222222222</v>
+        <v>42482.64722222222</v>
       </c>
       <c r="D51" s="1">
         <v>42482.654861111114</v>
       </c>
       <c r="E51" s="1">
-        <v>42482.655555555553</v>
+        <v>42482.65555555555</v>
       </c>
       <c r="F51" s="1">
         <v>42482.666666666664</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52">
       <c r="A52" s="1">
         <v>42496.63958333333</v>
       </c>
       <c r="B52" s="1">
-        <v>42496.648611111108</v>
+        <v>42496.64861111111</v>
       </c>
       <c r="C52" s="1">
         <v>42496.65</v>
       </c>
       <c r="D52" s="1">
-        <v>42496.668749999997</v>
+        <v>42496.66875</v>
       </c>
       <c r="E52" s="1">
-        <v>42496.673611111109</v>
+        <v>42496.67361111111</v>
       </c>
       <c r="F52" s="1">
-        <v>42496.673611111109</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42496.67361111111</v>
+      </c>
+    </row>
+    <row r="53">
       <c r="A53" s="1">
-        <v>42496.581250000003</v>
+        <v>42496.58125</v>
       </c>
       <c r="B53" s="1">
         <v>42496.59097222222</v>
@@ -1447,64 +1526,64 @@
         <v>42496.61041666667</v>
       </c>
       <c r="E53" s="1">
-        <v>42496.613194444442</v>
+        <v>42496.61319444444</v>
       </c>
       <c r="F53" s="1">
-        <v>42496.613194444442</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42496.61319444444</v>
+      </c>
+    </row>
+    <row r="54">
       <c r="A54" s="1">
         <v>42495.683333333334</v>
       </c>
       <c r="B54" s="1">
-        <v>42495.692361111112</v>
+        <v>42495.69236111111</v>
       </c>
       <c r="C54" s="1">
-        <v>42495.693055555559</v>
+        <v>42495.69305555556</v>
       </c>
       <c r="D54" s="1">
         <v>42495.70416666667</v>
       </c>
       <c r="E54" s="1">
-        <v>42495.712500000001</v>
+        <v>42495.7125</v>
       </c>
       <c r="F54" s="1">
-        <v>42495.718055555553</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42495.71805555555</v>
+      </c>
+    </row>
+    <row r="55">
       <c r="A55" s="1">
-        <v>42495.651388888888</v>
+        <v>42495.65138888889</v>
       </c>
       <c r="B55" s="1">
-        <v>42495.661111111112</v>
+        <v>42495.66111111111</v>
       </c>
       <c r="C55" s="1">
-        <v>42495.661805555559</v>
+        <v>42495.66180555556</v>
       </c>
       <c r="D55" s="1">
         <v>42495.669444444444</v>
       </c>
       <c r="E55" s="1">
-        <v>42495.679861111108</v>
+        <v>42495.67986111111</v>
       </c>
       <c r="F55" s="1">
-        <v>42495.679861111108</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42495.67986111111</v>
+      </c>
+    </row>
+    <row r="56">
       <c r="A56" s="1">
         <v>42495.618055555555</v>
       </c>
       <c r="B56" s="1">
-        <v>42495.627083333333</v>
+        <v>42495.62708333333</v>
       </c>
       <c r="C56" s="1">
         <v>42495.62777777778</v>
       </c>
       <c r="D56" s="1">
-        <v>42495.637499999997</v>
+        <v>42495.6375</v>
       </c>
       <c r="E56" s="1">
         <v>42495.649305555555</v>
@@ -1513,7 +1592,7 @@
         <v>42495.649305555555</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57">
       <c r="A57" s="1">
         <v>42495.592361111114</v>
       </c>
@@ -1527,33 +1606,33 @@
         <v>42495.606944444444</v>
       </c>
       <c r="E57" s="1">
-        <v>42495.612500000003</v>
+        <v>42495.6125</v>
       </c>
       <c r="F57" s="1">
-        <v>42495.612500000003</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42495.6125</v>
+      </c>
+    </row>
+    <row r="58">
       <c r="A58" s="1">
-        <v>42495.574305555558</v>
+        <v>42495.57430555556</v>
       </c>
       <c r="B58" s="1">
-        <v>42495.579861111109</v>
+        <v>42495.57986111111</v>
       </c>
       <c r="C58" s="1">
-        <v>42495.581250000003</v>
+        <v>42495.58125</v>
       </c>
       <c r="D58" s="1">
-        <v>42495.585416666669</v>
+        <v>42495.58541666667</v>
       </c>
       <c r="E58" s="1">
-        <v>42495.590277777781</v>
+        <v>42495.59027777778</v>
       </c>
       <c r="F58" s="1">
-        <v>42495.590277777781</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42495.59027777778</v>
+      </c>
+    </row>
+    <row r="59">
       <c r="A59" s="1">
         <v>42479.430555555555</v>
       </c>
@@ -1561,24 +1640,24 @@
         <v>42479.45</v>
       </c>
       <c r="C59" s="1">
-        <v>42479.453472222223</v>
+        <v>42479.45347222222</v>
       </c>
       <c r="D59" s="1">
-        <v>42479.465277777781</v>
+        <v>42479.46527777778</v>
       </c>
       <c r="E59" s="1">
-        <v>42479.477777777778</v>
+        <v>42479.47777777778</v>
       </c>
       <c r="F59" s="1">
-        <v>42479.477777777778</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42479.47777777778</v>
+      </c>
+    </row>
+    <row r="60">
       <c r="A60" s="1">
-        <v>42479.371527777781</v>
+        <v>42479.37152777778</v>
       </c>
       <c r="B60" s="1">
-        <v>42479.386111111111</v>
+        <v>42479.38611111111</v>
       </c>
       <c r="C60" s="1">
         <v>42479.388194444444</v>
@@ -1586,23 +1665,25 @@
       <c r="D60" s="1">
         <v>42479.404861111114</v>
       </c>
-      <c r="E60" s="1"/>
+      <c r="E60" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="F60" s="1">
-        <v>42479.425694444442</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42479.42569444444</v>
+      </c>
+    </row>
+    <row r="61">
       <c r="A61" s="1">
-        <v>42489.647916666669</v>
+        <v>42489.64791666667</v>
       </c>
       <c r="B61" s="1">
-        <v>42489.652777777781</v>
+        <v>42489.65277777778</v>
       </c>
       <c r="C61" s="1">
-        <v>42489.654166666667</v>
+        <v>42489.65416666667</v>
       </c>
       <c r="D61" s="1">
-        <v>42489.659722222219</v>
+        <v>42489.65972222222</v>
       </c>
       <c r="E61" s="1">
         <v>42489.663194444445</v>
@@ -1611,47 +1692,47 @@
         <v>42489.663194444445</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62">
       <c r="A62" s="1">
         <v>42489.626388888886</v>
       </c>
       <c r="B62" s="1">
-        <v>42489.631249999999</v>
+        <v>42489.63125</v>
       </c>
       <c r="C62" s="1">
-        <v>42489.642361111109</v>
+        <v>42489.64236111111</v>
       </c>
       <c r="D62" s="1">
         <v>42489.64166666667</v>
       </c>
       <c r="E62" s="1">
-        <v>42489.642361111109</v>
+        <v>42489.64236111111</v>
       </c>
       <c r="F62" s="1">
-        <v>42489.642361111109</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42489.64236111111</v>
+      </c>
+    </row>
+    <row r="63">
       <c r="A63" s="1">
-        <v>42489.588194444441</v>
+        <v>42489.58819444444</v>
       </c>
       <c r="B63" s="1">
         <v>42489.59375</v>
       </c>
       <c r="C63" s="1">
-        <v>42489.597222222219</v>
+        <v>42489.59722222222</v>
       </c>
       <c r="D63" s="1">
-        <v>42489.611111111109</v>
+        <v>42489.61111111111</v>
       </c>
       <c r="E63" s="1">
-        <v>42489.622916666667</v>
+        <v>42489.62291666667</v>
       </c>
       <c r="F63" s="1">
         <v>42489.638194444444</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64">
       <c r="A64" s="1">
         <v>42474.486805555556</v>
       </c>
@@ -1662,21 +1743,21 @@
         <v>42474.495833333334</v>
       </c>
       <c r="D64" s="1">
-        <v>42474.507638888892</v>
+        <v>42474.50763888889</v>
       </c>
       <c r="E64" s="1">
-        <v>42474.520138888889</v>
+        <v>42474.52013888889</v>
       </c>
       <c r="F64" s="1">
         <v>42474.520833333336</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65">
       <c r="A65" s="1">
-        <v>42474.459722222222</v>
+        <v>42474.45972222222</v>
       </c>
       <c r="B65" s="1">
-        <v>42474.465277777781</v>
+        <v>42474.46527777778</v>
       </c>
       <c r="C65" s="1">
         <v>42474.46875</v>
@@ -1688,30 +1769,30 @@
         <v>42474.48333333333</v>
       </c>
       <c r="F65" s="1">
-        <v>42474.484027777777</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+        <v>42474.48402777778</v>
+      </c>
+    </row>
+    <row r="66">
       <c r="A66" s="1">
         <v>42474.438888888886</v>
       </c>
       <c r="B66" s="1">
-        <v>42474.443749999999</v>
+        <v>42474.44375</v>
       </c>
       <c r="C66" s="1">
-        <v>42474.443749999999</v>
+        <v>42474.44375</v>
       </c>
       <c r="D66" s="1">
         <v>42474.45416666667</v>
       </c>
       <c r="E66" s="1">
-        <v>42474.454861111109</v>
+        <v>42474.45486111111</v>
       </c>
       <c r="F66" s="1">
         <v>42474.455555555556</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67">
       <c r="A67" s="1">
         <v>42474.415972222225</v>
       </c>
@@ -1725,7 +1806,7 @@
         <v>42474.424305555556</v>
       </c>
       <c r="E67" s="1">
-        <v>42474.429861111108</v>
+        <v>42474.42986111111</v>
       </c>
       <c r="F67" s="1">
         <v>42474.430555555555</v>
@@ -1733,5 +1814,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed missunderstanding with null cell input. Now adds the corresponding value to the adjasent cell
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Time of anaesthetic start</t>
   </si>
@@ -42,18 +42,6 @@
   </si>
   <si>
     <t>Time into Recovery</t>
-  </si>
-  <si>
-    <t>Time Out of Theatre</t>
-  </si>
-  <si>
-    <t>Time of Anaesthetic Start</t>
-  </si>
-  <si>
-    <t>Time into Theatre</t>
-  </si>
-  <si>
-    <t>Time out of Theatre</t>
   </si>
 </sst>
 </file>
@@ -493,8 +481,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
+      <c r="A2" s="3">
+        <v>42364.64861111111</v>
       </c>
       <c r="B2" s="1">
         <v>42364.64861111111</v>
@@ -508,8 +496,8 @@
       <c r="E2" s="1">
         <v>42364.68680555555</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
+      <c r="F2" s="3">
+        <v>42364.68680555555</v>
       </c>
     </row>
     <row r="3">
@@ -648,8 +636,8 @@
       <c r="E9" s="1">
         <v>42408.29027777778</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>6</v>
+      <c r="F9" s="3">
+        <v>42408.29027777778</v>
       </c>
     </row>
     <row r="10">
@@ -668,8 +656,8 @@
       <c r="E10" s="1">
         <v>42442.836805555555</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>6</v>
+      <c r="F10" s="3">
+        <v>42442.836805555555</v>
       </c>
     </row>
     <row r="11">
@@ -713,8 +701,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
-        <v>1</v>
+      <c r="A13" s="3">
+        <v>42464.381944444445</v>
       </c>
       <c r="B13" s="1">
         <v>42464.381944444445</v>
@@ -776,8 +764,8 @@
       <c r="A16" s="1">
         <v>42464.60208333333</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>7</v>
+      <c r="B16" s="3">
+        <v>42464.60208333333</v>
       </c>
       <c r="C16" s="1">
         <v>42464.6125</v>
@@ -899,8 +887,8 @@
       <c r="B22" s="1">
         <v>42468.58888888889</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>8</v>
+      <c r="C22" s="3">
+        <v>42468.58888888889</v>
       </c>
       <c r="D22" s="1">
         <v>42468.60208333333</v>
@@ -1128,8 +1116,8 @@
       <c r="E33" s="1">
         <v>42461.475694444445</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>6</v>
+      <c r="F33" s="3">
+        <v>42461.475694444445</v>
       </c>
     </row>
     <row r="34">
@@ -1273,8 +1261,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="3" t="s">
-        <v>1</v>
+      <c r="A41" s="3">
+        <v>42447.64375</v>
       </c>
       <c r="B41" s="1">
         <v>42447.64375</v>
@@ -1342,8 +1330,8 @@
       <c r="C44" s="1">
         <v>42481.72222222222</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>9</v>
+      <c r="D44" s="3">
+        <v>42481.74722222222</v>
       </c>
       <c r="E44" s="1">
         <v>42481.74722222222</v>
@@ -1425,8 +1413,8 @@
       <c r="D48" s="1">
         <v>42481.586805555555</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>5</v>
+      <c r="E48" s="3">
+        <v>42481.589583333334</v>
       </c>
       <c r="F48" s="1">
         <v>42481.589583333334</v>
@@ -1665,8 +1653,8 @@
       <c r="D60" s="1">
         <v>42479.404861111114</v>
       </c>
-      <c r="E60" s="3" t="s">
-        <v>5</v>
+      <c r="E60" s="3">
+        <v>42479.42569444444</v>
       </c>
       <c r="F60" s="1">
         <v>42479.42569444444</v>

</xml_diff>